<commit_message>
Se completa planilla de revisión
</commit_message>
<xml_diff>
--- a/Revisión Folino/1.4.Plantilla de revisión de PCBs - Folino.xlsx
+++ b/Revisión Folino/1.4.Plantilla de revisión de PCBs - Folino.xlsx
@@ -490,9 +490,6 @@
     <t>Sin observaciones</t>
   </si>
   <si>
-    <t>su libre uso</t>
-  </si>
-  <si>
     <t>La diagramación es prolija</t>
   </si>
   <si>
@@ -521,6 +518,9 @@
   </si>
   <si>
     <t>El esquematico es claro con las funciones bien delimitadas por sectores.</t>
+  </si>
+  <si>
+    <t>sin licencia de uso</t>
   </si>
 </sst>
 </file>
@@ -706,23 +706,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -736,6 +719,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1036,8 +1036,8 @@
   </sheetPr>
   <dimension ref="A1:D1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1048,20 +1048,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="3" t="s">
         <v>148</v>
       </c>
@@ -1070,31 +1070,31 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="11" t="s">
         <v>149</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="13.5">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="13" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="23" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="14" t="s">
         <v>151</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1102,21 +1102,21 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.5">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="13" t="s">
         <v>150</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="21">
+      <c r="B7" s="17"/>
+      <c r="C7" s="12">
         <v>44293</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1124,35 +1124,35 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="51.75">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="21">
+      <c r="B8" s="17"/>
+      <c r="C8" s="12">
         <v>44293</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:4" ht="13.5">
+      <c r="A9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="14"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="18" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="13" t="s">
         <v>152</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1160,11 +1160,11 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A11" s="18"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="13" t="s">
         <v>153</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1172,13 +1172,13 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="15" t="s">
         <v>150</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1186,11 +1186,11 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A13" s="18"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="15" t="s">
         <v>154</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1198,13 +1198,13 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="15" t="s">
         <v>156</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1212,11 +1212,11 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A15" s="17"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="15" t="s">
         <v>152</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1224,11 +1224,11 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A16" s="17"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="15" t="s">
         <v>155</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1236,23 +1236,23 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A17" s="17"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="C17" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A18" s="17"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="15" t="s">
         <v>157</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1260,127 +1260,127 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A19" s="17"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="24" t="s">
-        <v>159</v>
+      <c r="C19" s="15" t="s">
+        <v>158</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A20" s="17"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>160</v>
+      <c r="C20" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A21" s="17"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="24" t="s">
-        <v>160</v>
+      <c r="C21" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A22" s="17"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="24" t="s">
-        <v>161</v>
+      <c r="C22" s="15" t="s">
+        <v>160</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A23" s="17"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="24" t="s">
-        <v>162</v>
+      <c r="C23" s="15" t="s">
+        <v>161</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A24" s="17"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="24" t="s">
-        <v>163</v>
+      <c r="C24" s="15" t="s">
+        <v>162</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A25" s="17"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="24" t="s">
-        <v>164</v>
+      <c r="C25" s="15" t="s">
+        <v>163</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A26" s="17"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="24" t="s">
-        <v>165</v>
+      <c r="C26" s="15" t="s">
+        <v>164</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A27" s="17"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="24" t="s">
-        <v>167</v>
+      <c r="C27" s="15" t="s">
+        <v>166</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A28" s="17"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="24" t="s">
-        <v>168</v>
+      <c r="C28" s="15" t="s">
+        <v>167</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A29" s="17"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="4" t="s">
         <v>55</v>
       </c>
@@ -1388,7 +1388,7 @@
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A30" s="18"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="4" t="s">
         <v>56</v>
       </c>
@@ -1396,33 +1396,33 @@
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="18" t="s">
         <v>57</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="24" t="s">
-        <v>166</v>
+      <c r="C31" s="15" t="s">
+        <v>165</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A32" s="17"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="24" t="s">
-        <v>164</v>
+      <c r="C32" s="15" t="s">
+        <v>163</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="18" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -1434,7 +1434,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A34" s="17"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="4" t="s">
         <v>65</v>
       </c>
@@ -1444,7 +1444,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A35" s="17"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="4" t="s">
         <v>67</v>
       </c>
@@ -1454,7 +1454,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A36" s="18"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="4" t="s">
         <v>69</v>
       </c>
@@ -1464,7 +1464,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B37" s="6" t="s">
@@ -1476,7 +1476,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A38" s="17"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="5" t="s">
         <v>74</v>
       </c>
@@ -1486,7 +1486,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A39" s="17"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="4" t="s">
         <v>76</v>
       </c>
@@ -1496,7 +1496,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A40" s="17"/>
+      <c r="A40" s="19"/>
       <c r="B40" s="4" t="s">
         <v>78</v>
       </c>
@@ -1506,7 +1506,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A41" s="17"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="4" t="s">
         <v>80</v>
       </c>
@@ -1516,7 +1516,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A42" s="17"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="4" t="s">
         <v>82</v>
       </c>
@@ -1526,7 +1526,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A43" s="17"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="4" t="s">
         <v>84</v>
       </c>
@@ -1536,7 +1536,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A44" s="17"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="4" t="s">
         <v>86</v>
       </c>
@@ -1546,7 +1546,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A45" s="17"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="4" t="s">
         <v>88</v>
       </c>
@@ -1556,7 +1556,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A46" s="17"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="4" t="s">
         <v>90</v>
       </c>
@@ -1566,7 +1566,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A47" s="17"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="4" t="s">
         <v>92</v>
       </c>
@@ -1576,7 +1576,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A48" s="17"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="4" t="s">
         <v>94</v>
       </c>
@@ -1586,7 +1586,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A49" s="17"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="4" t="s">
         <v>96</v>
       </c>
@@ -1596,7 +1596,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A50" s="17"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="4" t="s">
         <v>98</v>
       </c>
@@ -1606,7 +1606,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A51" s="17"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="4" t="s">
         <v>100</v>
       </c>
@@ -1616,7 +1616,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A52" s="17"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="4" t="s">
         <v>102</v>
       </c>
@@ -1626,7 +1626,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A53" s="17"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="4" t="s">
         <v>104</v>
       </c>
@@ -1636,7 +1636,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A54" s="17"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="5" t="s">
         <v>106</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A55" s="17"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="5" t="s">
         <v>108</v>
       </c>
@@ -1656,7 +1656,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A56" s="17"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="5" t="s">
         <v>110</v>
       </c>
@@ -1666,7 +1666,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A57" s="17"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="4" t="s">
         <v>112</v>
       </c>
@@ -1676,7 +1676,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A58" s="17"/>
+      <c r="A58" s="19"/>
       <c r="B58" s="4" t="s">
         <v>114</v>
       </c>
@@ -1686,7 +1686,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A59" s="17"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="4" t="s">
         <v>116</v>
       </c>
@@ -1696,7 +1696,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A60" s="17"/>
+      <c r="A60" s="19"/>
       <c r="B60" s="4" t="s">
         <v>118</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A61" s="17"/>
+      <c r="A61" s="19"/>
       <c r="B61" s="4" t="s">
         <v>120</v>
       </c>
@@ -1716,7 +1716,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A62" s="17"/>
+      <c r="A62" s="19"/>
       <c r="B62" s="4" t="s">
         <v>122</v>
       </c>
@@ -1726,7 +1726,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A63" s="17"/>
+      <c r="A63" s="19"/>
       <c r="B63" s="4" t="s">
         <v>124</v>
       </c>
@@ -1736,7 +1736,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A64" s="17"/>
+      <c r="A64" s="19"/>
       <c r="B64" s="4" t="s">
         <v>126</v>
       </c>
@@ -1746,7 +1746,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A65" s="17"/>
+      <c r="A65" s="19"/>
       <c r="B65" s="4" t="s">
         <v>128</v>
       </c>
@@ -1756,7 +1756,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A66" s="17"/>
+      <c r="A66" s="19"/>
       <c r="B66" s="4" t="s">
         <v>130</v>
       </c>
@@ -1766,7 +1766,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A67" s="17"/>
+      <c r="A67" s="19"/>
       <c r="B67" s="4" t="s">
         <v>132</v>
       </c>
@@ -1776,7 +1776,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A68" s="17"/>
+      <c r="A68" s="19"/>
       <c r="B68" s="4" t="s">
         <v>134</v>
       </c>
@@ -1786,7 +1786,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A69" s="17"/>
+      <c r="A69" s="19"/>
       <c r="B69" s="4" t="s">
         <v>136</v>
       </c>
@@ -1796,7 +1796,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A70" s="17"/>
+      <c r="A70" s="19"/>
       <c r="B70" s="4" t="s">
         <v>138</v>
       </c>
@@ -1806,7 +1806,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A71" s="17"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="4" t="s">
         <v>140</v>
       </c>
@@ -1814,7 +1814,7 @@
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A72" s="18"/>
+      <c r="A72" s="20"/>
       <c r="B72" s="4" t="s">
         <v>141</v>
       </c>
@@ -1822,7 +1822,7 @@
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A73" s="19" t="s">
+      <c r="A73" s="21" t="s">
         <v>142</v>
       </c>
       <c r="B73" s="4" t="s">
@@ -1832,7 +1832,7 @@
       <c r="D73" s="9"/>
     </row>
     <row r="74" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A74" s="17"/>
+      <c r="A74" s="19"/>
       <c r="B74" s="4" t="s">
         <v>144</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="D74" s="9"/>
     </row>
     <row r="75" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A75" s="17"/>
+      <c r="A75" s="19"/>
       <c r="B75" s="4" t="s">
         <v>145</v>
       </c>
@@ -1848,7 +1848,7 @@
       <c r="D75" s="9"/>
     </row>
     <row r="76" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A76" s="17"/>
+      <c r="A76" s="19"/>
       <c r="B76" s="4" t="s">
         <v>146</v>
       </c>
@@ -1856,7 +1856,7 @@
       <c r="D76" s="9"/>
     </row>
     <row r="77" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A77" s="18"/>
+      <c r="A77" s="20"/>
       <c r="B77" s="5" t="s">
         <v>147</v>
       </c>
@@ -7577,6 +7577,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A37:A72"/>
@@ -7588,11 +7593,6 @@
     <mergeCell ref="A14:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1"/>

</xml_diff>